<commit_message>
Ready for final check
</commit_message>
<xml_diff>
--- a/inputData/Eco_FG.xlsx
+++ b/inputData/Eco_FG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10791792_polimi_it/Documents/2024-04 Economic model/EcoModel/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D6B61-07EB-4DB0-8EF1-29A5F1296ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{151D6B61-07EB-4DB0-8EF1-29A5F1296ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B86147E-4E8B-4694-B2AF-F0B226881EA6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>[-2.4   8.3  -11.2   5.2]'</t>
   </si>
@@ -61,9 +61,6 @@
     <t>structure.fixed.two.f_man</t>
   </si>
   <si>
-    <t>structure.soft.p_A</t>
-  </si>
-  <si>
     <t>f_mt</t>
   </si>
   <si>
@@ -97,24 +94,9 @@
     <t>winch.sigma_st</t>
   </si>
   <si>
-    <t>gearbox.approach</t>
-  </si>
-  <si>
     <t>structure.fixed.approach</t>
   </si>
   <si>
-    <t>gen.approach</t>
-  </si>
-  <si>
-    <t>pumpMotor.f_om</t>
-  </si>
-  <si>
-    <t>hydAccum.f_om</t>
-  </si>
-  <si>
-    <t>hydMotor.f_om</t>
-  </si>
-  <si>
     <t>sitePrep.p</t>
   </si>
   <si>
@@ -130,78 +112,24 @@
     <t>decomm.f</t>
   </si>
   <si>
-    <t>structure.soft.L_str</t>
-  </si>
-  <si>
     <t>obgen.p</t>
   </si>
   <si>
     <t>prop.p</t>
   </si>
   <si>
-    <t>avionics.C</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
-    <t>gearbox.one.p</t>
-  </si>
-  <si>
-    <t>gearbox.two.p</t>
-  </si>
-  <si>
-    <t>gearbox.two.k</t>
-  </si>
-  <si>
-    <t>gearbox.two.b</t>
-  </si>
-  <si>
-    <t>gen.one.p</t>
-  </si>
-  <si>
-    <t>gen.two.p</t>
-  </si>
-  <si>
-    <t>gen.two.b</t>
-  </si>
-  <si>
-    <t>gen.two.k</t>
-  </si>
-  <si>
     <t>ultracap.p</t>
   </si>
   <si>
     <t>ultracap.N</t>
   </si>
   <si>
-    <t>powerConv.p</t>
-  </si>
-  <si>
-    <t>pumpMotor.p_1</t>
-  </si>
-  <si>
-    <t>pumpMotor.p_2</t>
-  </si>
-  <si>
-    <t>hydAccum.p_1</t>
-  </si>
-  <si>
-    <t>hydAccum.p_2</t>
-  </si>
-  <si>
-    <t>hydMotor.p_1</t>
-  </si>
-  <si>
-    <t>hydMotor.p_2</t>
-  </si>
-  <si>
     <t>winch.material</t>
   </si>
   <si>
-    <t>drivetrain_type</t>
-  </si>
-  <si>
     <t>electricity.p_0</t>
   </si>
   <si>
@@ -218,6 +146,9 @@
   </si>
   <si>
     <t>N_bends</t>
+  </si>
+  <si>
+    <t>avio.C</t>
   </si>
 </sst>
 </file>
@@ -225,8 +156,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -263,12 +194,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -552,25 +483,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B3DA40-233C-46C9-8316-C78F88E0B4B1}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -578,7 +509,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -586,7 +517,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -594,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -602,7 +533,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -610,55 +541,39 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
     </row>
   </sheetData>
@@ -674,73 +589,73 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1">
         <v>80</v>
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>2.5</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>2.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -753,266 +668,104 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>7850</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="1">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21">
         <f>1000000</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31">
-        <v>8.3000000000000004E-2</v>
-      </c>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1028,46 +781,46 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>0.5</v>
@@ -1086,7 +839,7 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1100,30 +853,30 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B1">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>-1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>50</v>

</xml_diff>

<commit_message>
Update nomenclature. Clean code.
</commit_message>
<xml_diff>
--- a/inputData/Eco_FG.xlsx
+++ b/inputData/Eco_FG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10791792_polimi_it/Documents/2024-04 Economic model/EcoModel/inputData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{151D6B61-07EB-4DB0-8EF1-29A5F1296ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED315653-03D8-4A3F-BAF2-68F2F36A410E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F3B95E-BD25-4882-A4FB-698F1C25351E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-3525" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>[-2.4   8.3  -11.2   5.2]'</t>
   </si>
@@ -112,12 +112,6 @@
     <t>decomm.f</t>
   </si>
   <si>
-    <t>obgen.p</t>
-  </si>
-  <si>
-    <t>prop.p</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>avio.C</t>
   </si>
   <si>
-    <t>sigma</t>
-  </si>
-  <si>
     <t>winch.SF_Lt</t>
   </si>
   <si>
@@ -161,6 +152,12 @@
   </si>
   <si>
     <t>powerConv.p</t>
+  </si>
+  <si>
+    <t>obGen.p</t>
+  </si>
+  <si>
+    <t>sigma_max</t>
   </si>
 </sst>
 </file>
@@ -168,8 +165,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -206,12 +203,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -493,19 +490,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B3DA40-233C-46C9-8316-C78F88E0B4B1}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -513,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -521,7 +518,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -529,7 +526,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -537,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -545,7 +542,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -553,40 +550,24 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="1">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1">
         <v>15000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -597,26 +578,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4AD09E-FDEF-4026-AC1D-93146C2A9B86}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1">
         <v>80</v>
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -625,7 +606,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -633,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -641,7 +622,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -649,33 +630,33 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>2.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <f>1.5*10^9</f>
@@ -691,17 +672,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -709,7 +690,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -717,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -725,7 +706,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -734,7 +715,7 @@
         <v>300000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -742,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -750,7 +731,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -759,59 +740,59 @@
         <v>500000000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>60000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <f>1000000</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
   </sheetData>
@@ -828,12 +809,12 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -841,7 +822,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -849,7 +830,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -857,7 +838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -865,7 +846,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -886,7 +867,7 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -897,33 +878,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>-1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>50</v>

</xml_diff>